<commit_message>
feat: Import 6 months BB credit card history for ML training
- Added import script (scripts/import_bb_history.py) with:
  - BB category to system category mapping
  - Hash-based duplicate detection
  - Subscription keyword recognition

- Imported 665 transactions (Jul-Dec 2025)
  - Total: R$ 98,819.06
  - Categories: alimentacao, compras, assinaturas, saude, lazer, transporte, educacao

- Updated tracking files with latest data sync
- Added Esportes category for sports-related expenses

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 28/12/2025 19:35</t>
+          <t>Atualizado: 30/12/2025 18:33</t>
         </is>
       </c>
     </row>
@@ -1209,14 +1209,14 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>16500</v>
+        <v>21000</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0</v>
+        <v>29701.39</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>-100%</t>
+          <t>41%</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <v>9590</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>0</v>
+        <v>15798.61</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
@@ -1356,10 +1356,10 @@
         <v>4000</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>0</v>
+        <v>5048.87</v>
       </c>
       <c r="D14" s="13" t="n">
-        <v>0</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15">
@@ -1369,13 +1369,13 @@
         </is>
       </c>
       <c r="B15" s="6" t="n">
-        <v>1000</v>
+        <v>3500</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>0</v>
+        <v>8210.299999999999</v>
       </c>
       <c r="D15" s="13" t="n">
-        <v>0</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16">
@@ -1385,13 +1385,13 @@
         </is>
       </c>
       <c r="B16" s="6" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>0</v>
+        <v>9500</v>
       </c>
       <c r="D16" s="13" t="n">
-        <v>0</v>
+        <v>475</v>
       </c>
     </row>
     <row r="17">
@@ -1401,13 +1401,13 @@
         </is>
       </c>
       <c r="B17" s="6" t="n">
-        <v>3000</v>
+        <v>4200</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>0</v>
+        <v>222.91</v>
       </c>
       <c r="D17" s="13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -1417,13 +1417,13 @@
         </is>
       </c>
       <c r="B18" s="6" t="n">
-        <v>3000</v>
+        <v>3800</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>0</v>
+        <v>567.4</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
@@ -1433,13 +1433,13 @@
         </is>
       </c>
       <c r="B19" s="6" t="n">
-        <v>1500</v>
+        <v>1300</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>0</v>
+        <v>5493.15</v>
       </c>
       <c r="D19" s="13" t="n">
-        <v>0</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20">
@@ -1449,13 +1449,13 @@
         </is>
       </c>
       <c r="B20" s="6" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>0</v>
+        <v>618.86</v>
       </c>
       <c r="D20" s="13" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21">
@@ -1465,13 +1465,13 @@
         </is>
       </c>
       <c r="B21" s="6" t="n">
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="D21" s="13" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22">
@@ -1481,7 +1481,7 @@
         </is>
       </c>
       <c r="B22" s="6" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>0</v>
@@ -1607,7 +1607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1645,10 +1645,8 @@
           <t>Categoria</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Budget</t>
-        </is>
+      <c r="B4" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
@@ -1679,6 +1677,9 @@
         <is>
           <t>Jun</t>
         </is>
+      </c>
+      <c r="M4" t="n">
+        <v>5048.87</v>
       </c>
     </row>
     <row r="5">
@@ -1688,7 +1689,7 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>0</v>
@@ -1707,6 +1708,9 @@
       </c>
       <c r="H5" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>8210.299999999999</v>
       </c>
     </row>
     <row r="6">
@@ -1716,7 +1720,7 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>0</v>
@@ -1735,6 +1739,9 @@
       </c>
       <c r="H6" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>9500</v>
       </c>
     </row>
     <row r="7">
@@ -1744,7 +1751,7 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>0</v>
@@ -1763,6 +1770,9 @@
       </c>
       <c r="H7" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>222.91</v>
       </c>
     </row>
     <row r="8">
@@ -1772,7 +1782,7 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>0</v>
@@ -1791,6 +1801,9 @@
       </c>
       <c r="H8" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>567.4</v>
       </c>
     </row>
     <row r="9">
@@ -1800,7 +1813,7 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>0</v>
@@ -1819,6 +1832,9 @@
       </c>
       <c r="H9" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>5493.15</v>
       </c>
     </row>
     <row r="10">
@@ -1828,7 +1844,7 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>0</v>
@@ -1847,6 +1863,9 @@
       </c>
       <c r="H10" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>618.86</v>
       </c>
     </row>
     <row r="11">
@@ -1856,7 +1875,7 @@
         </is>
       </c>
       <c r="B11" s="6" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>0</v>
@@ -1875,6 +1894,9 @@
       </c>
       <c r="H11" s="6" t="n">
         <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>39.9</v>
       </c>
     </row>
     <row r="12">
@@ -1884,7 +1906,7 @@
         </is>
       </c>
       <c r="B12" s="6" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>0</v>
@@ -1902,6 +1924,9 @@
         <v>0</v>
       </c>
       <c r="H12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2042,20 +2067,14 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>Gasto Real</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>Disponível</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
+      <c r="C4" s="4" t="n">
+        <v>5048.87</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>-1048.87</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>1.2622175</v>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
@@ -2073,13 +2092,13 @@
         <v>4000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>0</v>
+        <v>8210.299999999999</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>4000</v>
+        <v>-4710.299999999999</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>0</v>
+        <v>2.3458</v>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
@@ -2097,13 +2116,13 @@
         <v>1000</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>0</v>
+        <v>9500</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>1000</v>
+        <v>-7500</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>0</v>
+        <v>4.75</v>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
@@ -2121,13 +2140,13 @@
         <v>1000</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0</v>
+        <v>222.91</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>1000</v>
+        <v>3977.09</v>
       </c>
       <c r="E7" s="18" t="n">
-        <v>0</v>
+        <v>0.05307380952380952</v>
       </c>
       <c r="F7" s="7" t="inlineStr">
         <is>
@@ -2145,13 +2164,13 @@
         <v>3000</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>0</v>
+        <v>567.4</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>3000</v>
+        <v>3232.6</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>0</v>
+        <v>0.1493157894736842</v>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
@@ -2169,13 +2188,13 @@
         <v>3000</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>0</v>
+        <v>5493.15</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>3000</v>
+        <v>-4193.15</v>
       </c>
       <c r="E9" s="18" t="n">
-        <v>0</v>
+        <v>4.225499999999999</v>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
@@ -2193,13 +2212,13 @@
         <v>1500</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>0</v>
+        <v>618.86</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>1500</v>
+        <v>881.14</v>
       </c>
       <c r="E10" s="18" t="n">
-        <v>0</v>
+        <v>0.4125733333333333</v>
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
@@ -2217,13 +2236,13 @@
         <v>500</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>500</v>
+        <v>360.1</v>
       </c>
       <c r="E11" s="18" t="n">
-        <v>0</v>
+        <v>0.09974999999999999</v>
       </c>
       <c r="F11" s="7" t="inlineStr">
         <is>
@@ -2244,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>2000</v>
+        <v>300</v>
       </c>
       <c r="E12" s="18" t="n">
         <v>0</v>
@@ -3480,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-28T19:35:42.501703</t>
+          <t>2025-12-30T18:33:45.564073</t>
         </is>
       </c>
     </row>
@@ -3538,7 +3557,7 @@
         <v>4000</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5048.87</v>
       </c>
     </row>
     <row r="9">
@@ -3554,7 +3573,7 @@
         <v>1000</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>8210.299999999999</v>
       </c>
     </row>
     <row r="10">
@@ -3570,7 +3589,7 @@
         <v>1000</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="11">
@@ -3586,7 +3605,7 @@
         <v>3000</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>222.91</v>
       </c>
     </row>
     <row r="12">
@@ -3602,7 +3621,7 @@
         <v>3000</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>567.4</v>
       </c>
     </row>
     <row r="13">
@@ -3618,7 +3637,7 @@
         <v>1500</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>5493.15</v>
       </c>
     </row>
     <row r="14">
@@ -3634,7 +3653,7 @@
         <v>500</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>618.86</v>
       </c>
     </row>
     <row r="15">
@@ -3650,7 +3669,7 @@
         <v>2000</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>39.9</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
feat: Add health insurance and utility bills from PicPay
- Added 6 months of health insurance payments (~R$1,400/month on day 10)
- Added utility bills: LIGHT (electricity), SAAE (water), AMPLA (gas)
- Updated import script to handle PicPay transactions:
  - Utilities (LIGHT, SAAE, AMPLA) → casa
  - Personal transfers (Karl Hackel, etc.) → ignored
- Removed blanket PICPAY* ignore pattern

New totals:
- Saude: R$3,516 → R$11,916 (+R$8,400)
- Casa: R$0 → R$1,332

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 30/12/2025 18:33</t>
+          <t>Atualizado: 30/12/2025 21:49</t>
         </is>
       </c>
     </row>
@@ -1212,11 +1212,11 @@
         <v>21000</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>29701.39</v>
+        <v>31101.39000000001</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>41%</t>
+          <t>48%</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <v>9590</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>15798.61</v>
+        <v>14398.60999999999</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
@@ -1372,10 +1372,10 @@
         <v>3500</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>8210.299999999999</v>
+        <v>7882.21</v>
       </c>
       <c r="D15" s="13" t="n">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16">
@@ -1404,10 +1404,10 @@
         <v>4200</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>222.91</v>
+        <v>3492.91</v>
       </c>
       <c r="D17" s="13" t="n">
-        <v>5</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18">
@@ -1420,10 +1420,10 @@
         <v>3800</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>567.4</v>
+        <v>1967.4</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19">
@@ -1436,10 +1436,10 @@
         <v>1300</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>5493.15</v>
+        <v>2551.24</v>
       </c>
       <c r="D19" s="13" t="n">
-        <v>422</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20">
@@ -1710,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>8210.299999999999</v>
+        <v>7882.21</v>
       </c>
     </row>
     <row r="6">
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>222.91</v>
+        <v>3492.91</v>
       </c>
     </row>
     <row r="8">
@@ -1803,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>567.4</v>
+        <v>1967.4</v>
       </c>
     </row>
     <row r="9">
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>5493.15</v>
+        <v>2551.24</v>
       </c>
     </row>
     <row r="10">
@@ -2092,13 +2092,13 @@
         <v>4000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>8210.299999999999</v>
+        <v>7882.21</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-4710.299999999999</v>
+        <v>-4382.21</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>2.3458</v>
+        <v>2.25206</v>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
@@ -2140,13 +2140,13 @@
         <v>1000</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>222.91</v>
+        <v>3492.91</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>3977.09</v>
+        <v>707.0900000000001</v>
       </c>
       <c r="E7" s="18" t="n">
-        <v>0.05307380952380952</v>
+        <v>0.831645238095238</v>
       </c>
       <c r="F7" s="7" t="inlineStr">
         <is>
@@ -2164,13 +2164,13 @@
         <v>3000</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>567.4</v>
+        <v>1967.4</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>3232.6</v>
+        <v>1832.6</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>0.1493157894736842</v>
+        <v>0.5177368421052632</v>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
@@ -2188,13 +2188,13 @@
         <v>3000</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>5493.15</v>
+        <v>2551.24</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>-4193.15</v>
+        <v>-1251.24</v>
       </c>
       <c r="E9" s="18" t="n">
-        <v>4.225499999999999</v>
+        <v>1.962492307692308</v>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-30T18:33:45.564073</t>
+          <t>2025-12-30T21:49:28.626440</t>
         </is>
       </c>
     </row>
@@ -3573,7 +3573,7 @@
         <v>1000</v>
       </c>
       <c r="D9" t="n">
-        <v>8210.299999999999</v>
+        <v>7882.21</v>
       </c>
     </row>
     <row r="10">
@@ -3605,7 +3605,7 @@
         <v>3000</v>
       </c>
       <c r="D11" t="n">
-        <v>222.91</v>
+        <v>3492.91</v>
       </c>
     </row>
     <row r="12">
@@ -3621,7 +3621,7 @@
         <v>3000</v>
       </c>
       <c r="D12" t="n">
-        <v>567.4</v>
+        <v>1967.4</v>
       </c>
     </row>
     <row r="13">
@@ -3637,7 +3637,7 @@
         <v>1500</v>
       </c>
       <c r="D13" t="n">
-        <v>5493.15</v>
+        <v>2551.24</v>
       </c>
     </row>
     <row r="14">

</xml_diff>

<commit_message>
feat: Adjust budgets based on 6-month real spending data
Budget changes:
- alimentacao: R$4,000 → R$3,500
- compras: R$3,500 → R$2,500
- transporte: R$4,200 → R$4,000
- assinaturas: R$1,300 → R$3,500 (reflect actual SaaS spending)
- saude: R$3,800 → R$2,000
- casa: R$2,000 → R$500 (utilities only)
- taxas: R$300 → R$100
- educacao: R$400 → R$200

Total monthly budget: R$21,000 → R$17,800

Also added tennis/sports keywords to import script for lazer category.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 30/12/2025 21:49</t>
+          <t>Atualizado: 30/12/2025 21:59</t>
         </is>
       </c>
     </row>
@@ -1209,14 +1209,14 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>21000</v>
+        <v>17800</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>31101.39000000001</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>48%</t>
+          <t>74%</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -1353,13 +1353,13 @@
         </is>
       </c>
       <c r="B14" s="6" t="n">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>5048.87</v>
       </c>
       <c r="D14" s="13" t="n">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15">
@@ -1369,13 +1369,13 @@
         </is>
       </c>
       <c r="B15" s="6" t="n">
-        <v>3500</v>
+        <v>2500</v>
       </c>
       <c r="C15" s="6" t="n">
         <v>7882.21</v>
       </c>
       <c r="D15" s="13" t="n">
-        <v>225</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16">
@@ -1385,13 +1385,13 @@
         </is>
       </c>
       <c r="B16" s="6" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>9500</v>
       </c>
       <c r="D16" s="13" t="n">
-        <v>475</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="17">
@@ -1401,13 +1401,13 @@
         </is>
       </c>
       <c r="B17" s="6" t="n">
-        <v>4200</v>
+        <v>4000</v>
       </c>
       <c r="C17" s="6" t="n">
         <v>3492.91</v>
       </c>
       <c r="D17" s="13" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18">
@@ -1417,13 +1417,13 @@
         </is>
       </c>
       <c r="B18" s="6" t="n">
-        <v>3800</v>
+        <v>2000</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>1967.4</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>51</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -1433,13 +1433,13 @@
         </is>
       </c>
       <c r="B19" s="6" t="n">
-        <v>1300</v>
+        <v>3500</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>2551.24</v>
       </c>
       <c r="D19" s="13" t="n">
-        <v>196</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
@@ -1465,13 +1465,13 @@
         </is>
       </c>
       <c r="B21" s="6" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>39.9</v>
       </c>
       <c r="D21" s="13" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -1481,7 +1481,7 @@
         </is>
       </c>
       <c r="B22" s="6" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>0</v>
@@ -2071,10 +2071,10 @@
         <v>5048.87</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>-1048.87</v>
+        <v>-1548.87</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>1.2622175</v>
+        <v>1.442534285714286</v>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
@@ -2095,10 +2095,10 @@
         <v>7882.21</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-4382.21</v>
+        <v>-5382.21</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>2.25206</v>
+        <v>3.152884</v>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
@@ -2119,10 +2119,10 @@
         <v>9500</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>-7500</v>
+        <v>-9000</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>4.75</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
@@ -2143,10 +2143,10 @@
         <v>3492.91</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>707.0900000000001</v>
+        <v>507.0900000000001</v>
       </c>
       <c r="E7" s="18" t="n">
-        <v>0.831645238095238</v>
+        <v>0.8732274999999999</v>
       </c>
       <c r="F7" s="7" t="inlineStr">
         <is>
@@ -2167,10 +2167,10 @@
         <v>1967.4</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>1832.6</v>
+        <v>32.59999999999991</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>0.5177368421052632</v>
+        <v>0.9837</v>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
@@ -2191,10 +2191,10 @@
         <v>2551.24</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>-1251.24</v>
+        <v>948.7599999999998</v>
       </c>
       <c r="E9" s="18" t="n">
-        <v>1.962492307692308</v>
+        <v>0.7289257142857144</v>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
@@ -2239,10 +2239,10 @@
         <v>39.9</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>360.1</v>
+        <v>160.1</v>
       </c>
       <c r="E11" s="18" t="n">
-        <v>0.09974999999999999</v>
+        <v>0.1995</v>
       </c>
       <c r="F11" s="7" t="inlineStr">
         <is>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E12" s="18" t="n">
         <v>0</v>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-30T21:49:28.626440</t>
+          <t>2025-12-30T21:59:11.964253</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Gerar transações automáticas de parcelamentos no budget
Adiciona função generate_installment_transactions() que:
- Gera transações para cada parcelamento ativo no mês especificado
- Calcula automaticamente o número da parcela (2/10, 3/10, etc.)
- Usa hash para evitar duplicatas
- Integrado ao sync_all() para gerar antes de sincronizar

Isso garante que os parcelamentos "comam" do budget mensal e
apareçam nos dashboards corretamente.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 30/12/2025 21:59</t>
+          <t>Atualizado: 30/12/2025 22:06</t>
         </is>
       </c>
     </row>
@@ -1212,11 +1212,11 @@
         <v>17800</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>31101.39000000001</v>
+        <v>20365.58</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>74%</t>
+          <t>14%</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <v>9590</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>14398.60999999999</v>
+        <v>25134.42</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
@@ -1356,10 +1356,10 @@
         <v>3500</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>5048.87</v>
+        <v>0</v>
       </c>
       <c r="D14" s="13" t="n">
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1372,10 +1372,10 @@
         <v>2500</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>7882.21</v>
+        <v>2110.74</v>
       </c>
       <c r="D15" s="13" t="n">
-        <v>315</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16">
@@ -1388,10 +1388,10 @@
         <v>500</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>9500</v>
+        <v>12830.24</v>
       </c>
       <c r="D16" s="13" t="n">
-        <v>1900</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="17">
@@ -1404,10 +1404,10 @@
         <v>4000</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>3492.91</v>
+        <v>0</v>
       </c>
       <c r="D17" s="13" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1420,10 +1420,10 @@
         <v>2000</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>1967.4</v>
+        <v>4669.66</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>98</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19">
@@ -1436,10 +1436,10 @@
         <v>3500</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>2551.24</v>
+        <v>754.9400000000001</v>
       </c>
       <c r="D19" s="13" t="n">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20">
@@ -1452,10 +1452,10 @@
         <v>1500</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>618.86</v>
+        <v>0</v>
       </c>
       <c r="D20" s="13" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1468,10 +1468,10 @@
         <v>200</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>39.9</v>
+        <v>0</v>
       </c>
       <c r="D21" s="13" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1689,7 +1689,7 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>0</v>
+        <v>2110.74</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>0</v>
@@ -1720,7 +1720,7 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>0</v>
+        <v>12830.24</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>0</v>
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>0</v>
+        <v>4669.66</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>0</v>
@@ -1813,7 +1813,7 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>0</v>
+        <v>754.9400000000001</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>0</v>
@@ -2068,13 +2068,13 @@
         </is>
       </c>
       <c r="C4" s="4" t="n">
-        <v>5048.87</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>-1548.87</v>
+        <v>3500</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>1.442534285714286</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
@@ -2092,13 +2092,13 @@
         <v>4000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>7882.21</v>
+        <v>2110.74</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>-5382.21</v>
+        <v>389.2599999999998</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>3.152884</v>
+        <v>0.844296</v>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
@@ -2116,13 +2116,13 @@
         <v>1000</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>9500</v>
+        <v>12830.24</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>-9000</v>
+        <v>-12330.24</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>19</v>
+        <v>25.66048</v>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
@@ -2140,13 +2140,13 @@
         <v>1000</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>3492.91</v>
+        <v>0</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>507.0900000000001</v>
+        <v>4000</v>
       </c>
       <c r="E7" s="18" t="n">
-        <v>0.8732274999999999</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7" t="inlineStr">
         <is>
@@ -2164,13 +2164,13 @@
         <v>3000</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>1967.4</v>
+        <v>4669.66</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>32.59999999999991</v>
+        <v>-2669.66</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>0.9837</v>
+        <v>2.33483</v>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
@@ -2188,13 +2188,13 @@
         <v>3000</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>2551.24</v>
+        <v>754.9400000000001</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>948.7599999999998</v>
+        <v>2745.06</v>
       </c>
       <c r="E9" s="18" t="n">
-        <v>0.7289257142857144</v>
+        <v>0.2156971428571429</v>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
@@ -2212,13 +2212,13 @@
         <v>1500</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>618.86</v>
+        <v>0</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>881.14</v>
+        <v>1500</v>
       </c>
       <c r="E10" s="18" t="n">
-        <v>0.4125733333333333</v>
+        <v>0</v>
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
@@ -2236,13 +2236,13 @@
         <v>500</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>39.9</v>
+        <v>0</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>160.1</v>
+        <v>200</v>
       </c>
       <c r="E11" s="18" t="n">
-        <v>0.1995</v>
+        <v>0</v>
       </c>
       <c r="F11" s="7" t="inlineStr">
         <is>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-30T21:59:11.964253</t>
+          <t>2025-12-30T22:06:33.199886</t>
         </is>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
         <v>4000</v>
       </c>
       <c r="D8" t="n">
-        <v>5048.87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3573,7 +3573,7 @@
         <v>1000</v>
       </c>
       <c r="D9" t="n">
-        <v>7882.21</v>
+        <v>2110.74</v>
       </c>
     </row>
     <row r="10">
@@ -3589,7 +3589,7 @@
         <v>1000</v>
       </c>
       <c r="D10" t="n">
-        <v>9500</v>
+        <v>12830.24</v>
       </c>
     </row>
     <row r="11">
@@ -3605,7 +3605,7 @@
         <v>3000</v>
       </c>
       <c r="D11" t="n">
-        <v>3492.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -3621,7 +3621,7 @@
         <v>3000</v>
       </c>
       <c r="D12" t="n">
-        <v>1967.4</v>
+        <v>4669.66</v>
       </c>
     </row>
     <row r="13">
@@ -3637,7 +3637,7 @@
         <v>1500</v>
       </c>
       <c r="D13" t="n">
-        <v>2551.24</v>
+        <v>754.9400000000001</v>
       </c>
     </row>
     <row r="14">
@@ -3653,7 +3653,7 @@
         <v>500</v>
       </c>
       <c r="D14" t="n">
-        <v>618.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -3669,7 +3669,7 @@
         <v>2000</v>
       </c>
       <c r="D15" t="n">
-        <v>39.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
feat: Separar gastos de obra do budget mensal
- Criar categoria 'obra' (budget R$ 0) para construção/móveis
- Mover MOVEIS PLANEJADOS, ELETRODOMESTICOS, MESA E CADEIRAS para obra
- Dashboard exibe obra separadamente (não conta no budget variável)
- KPI "Obra" separado mostrando gastos de construção
- Corrigir divisão por zero quando budget = 0

Gastos de obra são mostrados mas não distorcem o acompanhamento
de budget mensal das despesas variáveis regulares.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 30/12/2025 22:06</t>
+          <t>Atualizado: 31/12/2025 11:09</t>
         </is>
       </c>
     </row>
@@ -1212,11 +1212,11 @@
         <v>17800</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>20365.58</v>
+        <v>9265.58</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>14%</t>
+          <t>-47%</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <v>9590</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>25134.42</v>
+        <v>36234.42</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
@@ -1388,10 +1388,10 @@
         <v>500</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>12830.24</v>
+        <v>1730.24</v>
       </c>
       <c r="D16" s="13" t="n">
-        <v>2566</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17">
@@ -1720,7 +1720,7 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>12830.24</v>
+        <v>1730.24</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>0</v>
@@ -2116,13 +2116,13 @@
         <v>1000</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>12830.24</v>
+        <v>1730.24</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>-12330.24</v>
+        <v>-1230.24</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>25.66048</v>
+        <v>3.46048</v>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-30T22:06:33.199886</t>
+          <t>2025-12-31T11:09:01.247836</t>
         </is>
       </c>
     </row>
@@ -3589,7 +3589,7 @@
         <v>1000</v>
       </c>
       <c r="D10" t="n">
-        <v>12830.24</v>
+        <v>1730.24</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
feat: Definir budget de obra como R$ 16.500/mês
Baseado na análise do cronograma de obra 2026:
- Total projeto: R$ 197.440
- Parcelamentos: R$ 116.500 (móveis, eletros)
- Obra física: R$ 80.940 (elétrica, piso, pintura)
- Média mensal: R$ 16.453 ≈ R$ 16.500

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 31/12/2025 11:09</t>
+          <t>Atualizado: 31/12/2025 11:15</t>
         </is>
       </c>
     </row>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-31T11:09:01.247836</t>
+          <t>2025-12-31T11:15:59.739453</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Remover TRATAMENTO EMAGRECIMENTO e ajustar budget saúde
- Remover TRATAMENTO EMAGRECIMENTO dos parcelamentos (era referência, não real)
- Atualizar budget saúde de R$ 2.000 para R$ 4.000
- Total gastos reduzido de R$ 20.365 para R$ 17.865 (-R$ 2.500)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 31/12/2025 11:15</t>
+          <t>Atualizado: 31/12/2025 11:23</t>
         </is>
       </c>
     </row>
@@ -1209,14 +1209,14 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>17800</v>
+        <v>19800</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>9265.58</v>
+        <v>6765.58</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>-47%</t>
+          <t>-65%</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <v>9590</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>36234.42</v>
+        <v>38734.42</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
@@ -1417,13 +1417,13 @@
         </is>
       </c>
       <c r="B18" s="6" t="n">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>4669.66</v>
+        <v>2169.66</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>233</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>4669.66</v>
+        <v>2169.66</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>0</v>
@@ -2164,13 +2164,13 @@
         <v>3000</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>4669.66</v>
+        <v>2169.66</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>-2669.66</v>
+        <v>1830.34</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>2.33483</v>
+        <v>0.542415</v>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-31T11:15:59.739453</t>
+          <t>2025-12-31T11:23:58.847300</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
         <v>3000</v>
       </c>
       <c r="D12" t="n">
-        <v>4669.66</v>
+        <v>2169.66</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
fix: Corrigir cálculo de poupança em sync_excel.py e regenerar relatórios
- Remover hardcode de R$ 9.500 (parcela MOVEIS duplicada removida)
- Calcular total de categorias excluídas (obra/esportes) dinamicamente do banco
- Atualizar Dashboard_2026.xlsx com dados corretos Janeiro 2026
- Regenerar todos os relatórios Obsidian (PF + PJ) com dados atualizados

Totais Janeiro 2026:
- Gastos Variáveis: R$ 21.602,84
- Gastos Obra/Esportes: R$ 11.166,90
- Taxa Poupança: 60,7%
- Poupança Excel: R$ 22.230,26
</commit_message>
<xml_diff>
--- a/projections/Dashboard_2026.xlsx
+++ b/projections/Dashboard_2026.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Dashboard" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Mensal" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Categorias" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Parcelamentos" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Fluxo Anual" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Previsões ML" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Dados" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dashboard" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mensal" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Categorias" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Parcelamentos" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Fluxo Anual" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Previsões ML" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dados" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -240,13 +240,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -270,7 +270,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -294,7 +294,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -322,8 +322,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -349,8 +349,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -376,13 +376,13 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -405,14 +405,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -437,14 +437,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -472,8 +472,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -499,8 +499,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -526,13 +526,13 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -555,7 +555,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -587,13 +587,13 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -616,14 +616,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -648,14 +648,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -695,8 +695,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -722,7 +722,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>5</col>
@@ -737,9 +737,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -759,9 +759,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -771,7 +771,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -786,9 +786,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -798,7 +798,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>13</col>
@@ -813,9 +813,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1141,7 +1141,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado: 31/12/2025 11:23</t>
+          <t>Atualizado: 25/01/2026 17:00</t>
         </is>
       </c>
     </row>
@@ -1209,14 +1209,14 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>19800</v>
+        <v>20700</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>6765.58</v>
+        <v>21602.84</v>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>-65%</t>
+          <t>4%</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
@@ -1258,7 +1258,7 @@
         <v>9590</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>38734.42</v>
+        <v>22230.26</v>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
@@ -1356,10 +1356,10 @@
         <v>3500</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>0</v>
+        <v>2942.2</v>
       </c>
       <c r="D14" s="13" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
@@ -1372,10 +1372,10 @@
         <v>2500</v>
       </c>
       <c r="C15" s="6" t="n">
-        <v>2110.74</v>
+        <v>3166.83</v>
       </c>
       <c r="D15" s="13" t="n">
-        <v>84</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16">
@@ -1388,10 +1388,10 @@
         <v>500</v>
       </c>
       <c r="C16" s="6" t="n">
-        <v>1730.24</v>
+        <v>393</v>
       </c>
       <c r="D16" s="13" t="n">
-        <v>346</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
@@ -1404,10 +1404,10 @@
         <v>4000</v>
       </c>
       <c r="C17" s="6" t="n">
-        <v>0</v>
+        <v>3685.44</v>
       </c>
       <c r="D17" s="13" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
@@ -1420,10 +1420,10 @@
         <v>4000</v>
       </c>
       <c r="C18" s="6" t="n">
-        <v>2169.66</v>
+        <v>4624.690000000001</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>54</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19">
@@ -1436,10 +1436,10 @@
         <v>3500</v>
       </c>
       <c r="C19" s="6" t="n">
-        <v>754.9400000000001</v>
+        <v>4021.1</v>
       </c>
       <c r="D19" s="13" t="n">
-        <v>21</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20">
@@ -1452,10 +1452,10 @@
         <v>1500</v>
       </c>
       <c r="C20" s="6" t="n">
-        <v>0</v>
+        <v>1563.33</v>
       </c>
       <c r="D20" s="13" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
@@ -1468,10 +1468,10 @@
         <v>200</v>
       </c>
       <c r="C21" s="6" t="n">
-        <v>0</v>
+        <v>163.84</v>
       </c>
       <c r="D21" s="13" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22">
@@ -1481,13 +1481,13 @@
         </is>
       </c>
       <c r="B22" s="6" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C22" s="6" t="n">
-        <v>0</v>
+        <v>1042.41</v>
       </c>
       <c r="D22" s="13" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25">
@@ -1646,7 +1646,7 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0</v>
+        <v>2942.2</v>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
@@ -1689,7 +1689,7 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>2110.74</v>
+        <v>3166.83</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>0</v>
@@ -1720,7 +1720,7 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>1730.24</v>
+        <v>393</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>0</v>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>0</v>
+        <v>3685.44</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>0</v>
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>2169.66</v>
+        <v>4624.690000000001</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>0</v>
@@ -1813,7 +1813,7 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>754.9400000000001</v>
+        <v>4021.1</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>0</v>
@@ -1844,7 +1844,7 @@
         </is>
       </c>
       <c r="B10" s="6" t="n">
-        <v>0</v>
+        <v>1563.33</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>0</v>
@@ -1875,7 +1875,7 @@
         </is>
       </c>
       <c r="B11" s="6" t="n">
-        <v>0</v>
+        <v>163.84</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>0</v>
@@ -1906,7 +1906,7 @@
         </is>
       </c>
       <c r="B12" s="6" t="n">
-        <v>0</v>
+        <v>1042.41</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>0</v>
@@ -2068,13 +2068,13 @@
         </is>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0</v>
+        <v>2942.2</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>3500</v>
+        <v>557.8000000000002</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0</v>
+        <v>0.8406285714285714</v>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
@@ -2092,13 +2092,13 @@
         <v>4000</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>2110.74</v>
+        <v>3166.83</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>389.2599999999998</v>
+        <v>-666.8299999999999</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>0.844296</v>
+        <v>1.266732</v>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
@@ -2116,13 +2116,13 @@
         <v>1000</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>1730.24</v>
+        <v>393</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>-1230.24</v>
+        <v>107</v>
       </c>
       <c r="E6" s="18" t="n">
-        <v>3.46048</v>
+        <v>0.786</v>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
@@ -2140,13 +2140,13 @@
         <v>1000</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0</v>
+        <v>3685.44</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>4000</v>
+        <v>314.5599999999999</v>
       </c>
       <c r="E7" s="18" t="n">
-        <v>0</v>
+        <v>0.9213600000000001</v>
       </c>
       <c r="F7" s="7" t="inlineStr">
         <is>
@@ -2164,13 +2164,13 @@
         <v>3000</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>2169.66</v>
+        <v>4624.690000000001</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>1830.34</v>
+        <v>-624.6900000000005</v>
       </c>
       <c r="E8" s="18" t="n">
-        <v>0.542415</v>
+        <v>1.1561725</v>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
@@ -2188,13 +2188,13 @@
         <v>3000</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>754.9400000000001</v>
+        <v>4021.1</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>2745.06</v>
+        <v>-521.0999999999999</v>
       </c>
       <c r="E9" s="18" t="n">
-        <v>0.2156971428571429</v>
+        <v>1.148885714285714</v>
       </c>
       <c r="F9" s="7" t="inlineStr">
         <is>
@@ -2212,13 +2212,13 @@
         <v>1500</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>0</v>
+        <v>1563.33</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>1500</v>
+        <v>-63.33000000000015</v>
       </c>
       <c r="E10" s="18" t="n">
-        <v>0</v>
+        <v>1.04222</v>
       </c>
       <c r="F10" s="7" t="inlineStr">
         <is>
@@ -2236,13 +2236,13 @@
         <v>500</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>0</v>
+        <v>163.84</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>200</v>
+        <v>36.16</v>
       </c>
       <c r="E11" s="18" t="n">
-        <v>0</v>
+        <v>0.8192</v>
       </c>
       <c r="F11" s="7" t="inlineStr">
         <is>
@@ -2260,13 +2260,13 @@
         <v>2000</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>0</v>
+        <v>1042.41</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>100</v>
+        <v>-42.41000000000008</v>
       </c>
       <c r="E12" s="18" t="n">
-        <v>0</v>
+        <v>1.04241</v>
       </c>
       <c r="F12" s="7" t="inlineStr">
         <is>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-12-31T11:23:58.847300</t>
+          <t>2026-01-25T17:00:59.990258</t>
         </is>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
         <v>4000</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>2942.2</v>
       </c>
     </row>
     <row r="9">
@@ -3573,7 +3573,7 @@
         <v>1000</v>
       </c>
       <c r="D9" t="n">
-        <v>2110.74</v>
+        <v>3166.83</v>
       </c>
     </row>
     <row r="10">
@@ -3589,7 +3589,7 @@
         <v>1000</v>
       </c>
       <c r="D10" t="n">
-        <v>1730.24</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11">
@@ -3605,7 +3605,7 @@
         <v>3000</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3685.44</v>
       </c>
     </row>
     <row r="12">
@@ -3621,7 +3621,7 @@
         <v>3000</v>
       </c>
       <c r="D12" t="n">
-        <v>2169.66</v>
+        <v>4624.690000000001</v>
       </c>
     </row>
     <row r="13">
@@ -3637,7 +3637,7 @@
         <v>1500</v>
       </c>
       <c r="D13" t="n">
-        <v>754.9400000000001</v>
+        <v>4021.1</v>
       </c>
     </row>
     <row r="14">
@@ -3653,7 +3653,7 @@
         <v>500</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1563.33</v>
       </c>
     </row>
     <row r="15">
@@ -3669,7 +3669,7 @@
         <v>2000</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>163.84</v>
       </c>
     </row>
     <row r="16">
@@ -3685,7 +3685,7 @@
         <v>500</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1042.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>